<commit_message>
Update of the tutorial
</commit_message>
<xml_diff>
--- a/Tutorial/enrichment_std.xlsx
+++ b/Tutorial/enrichment_std.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d717abb17622efd7/Work/Python notebooks/Alpaca_playground/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2DDF052A-902E-45C7-BEC4-B507EB46F090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF894CB9-F875-D942-BE79-9026D24DA063}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{2DDF052A-902E-45C7-BEC4-B507EB46F090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B347DCE-5D23-0C4E-8554-BC54E2B54681}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20160" windowHeight="9420" xr2:uid="{221DCA28-C690-4B94-9AF0-A3D954F17C7D}"/>
   </bookViews>
@@ -525,14 +525,14 @@
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
     <col min="6" max="6" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.33203125" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>